<commit_message>
fix: adding comment, and changing xlsx file
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\RPA\RPA-AP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3F98A1-433D-4F92-BC79-9849C93301F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FEC1F0-B11D-4501-B6DC-64E06DEF47DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Tarefa</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Digitar Senha</t>
-  </si>
-  <si>
-    <t>Harminda#2403</t>
   </si>
   <si>
     <t>Logout</t>
@@ -378,7 +375,7 @@
   <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -419,7 +416,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,9 +525,7 @@
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3">
-        <v>2303701</v>
-      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -572,9 +567,7 @@
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -655,13 +648,13 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>